<commit_message>
Feature: Dasboard refinado e enviando arquivo para otimização.
</commit_message>
<xml_diff>
--- a/src/APSSystem.Presentation.WPF/Data/Antecipacao/Recursos.xlsx
+++ b/src/APSSystem.Presentation.WPF/Data/Antecipacao/Recursos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55159\APSSystem\src\Presentation\Data\CenarioAntecipacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55159\source\repos\APSSystem_NOVO\src\APSSystem.Presentation.WPF\Data\Antecipacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DD5C73-98E9-4BAF-98AD-D77D6A335542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0ED9DE-E2E3-481F-AABB-E06F4154A948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31890" yWindow="4065" windowWidth="18180" windowHeight="9885" xr2:uid="{BE9E9A5A-8528-4279-9018-52A1C569EF13}"/>
   </bookViews>
@@ -444,10 +444,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC5CD8A-5F0F-4FD0-8B93-7C8E0EF73F21}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="A5" sqref="A5:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,11 +569,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F12">
-        <v>60</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
feature: melhorias na tela 2 antes de alterar grid
</commit_message>
<xml_diff>
--- a/src/APSSystem.Presentation.WPF/Data/Antecipacao/Recursos.xlsx
+++ b/src/APSSystem.Presentation.WPF/Data/Antecipacao/Recursos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55159\source\repos\APSSystem_NOVO\src\APSSystem.Presentation.WPF\Data\Antecipacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0ED9DE-E2E3-481F-AABB-E06F4154A948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039CA35D-CF98-4FAC-A4AC-843BA664525C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31890" yWindow="4065" windowWidth="18180" windowHeight="9885" xr2:uid="{BE9E9A5A-8528-4279-9018-52A1C569EF13}"/>
+    <workbookView xWindow="24345" yWindow="15810" windowWidth="18180" windowHeight="9885" xr2:uid="{BE9E9A5A-8528-4279-9018-52A1C569EF13}"/>
   </bookViews>
   <sheets>
     <sheet name="machine" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD17"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,8 +496,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="1">
-        <f>1000/60</f>
-        <v>16.666666666666668</v>
+        <v>1000</v>
       </c>
       <c r="D2">
         <v>0.9</v>
@@ -523,8 +522,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C4" si="0">1000/60</f>
-        <v>16.666666666666668</v>
+        <v>1000</v>
       </c>
       <c r="D3">
         <v>0.8</v>
@@ -550,8 +548,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
-        <v>16.666666666666668</v>
+        <v>1000</v>
       </c>
       <c r="D4">
         <v>0.7</v>

</xml_diff>

<commit_message>
feature: PoC v1.0 - falta atualizar tela1
</commit_message>
<xml_diff>
--- a/src/APSSystem.Presentation.WPF/Data/Antecipacao/Recursos.xlsx
+++ b/src/APSSystem.Presentation.WPF/Data/Antecipacao/Recursos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55159\source\repos\APSSystem_NOVO\src\APSSystem.Presentation.WPF\Data\Antecipacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039CA35D-CF98-4FAC-A4AC-843BA664525C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D75A986-62DA-4878-8F98-8B1395E07609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24345" yWindow="15810" windowWidth="18180" windowHeight="9885" xr2:uid="{BE9E9A5A-8528-4279-9018-52A1C569EF13}"/>
+    <workbookView xWindow="34905" yWindow="5490" windowWidth="22320" windowHeight="15300" xr2:uid="{BE9E9A5A-8528-4279-9018-52A1C569EF13}"/>
   </bookViews>
   <sheets>
     <sheet name="machine" sheetId="1" r:id="rId1"/>
@@ -79,8 +79,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -127,7 +128,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +448,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feature: PoC v1.2.0 - Versão final da Prova de Conceito para deployment
</commit_message>
<xml_diff>
--- a/src/APSSystem.Presentation.WPF/Data/Antecipacao/Recursos.xlsx
+++ b/src/APSSystem.Presentation.WPF/Data/Antecipacao/Recursos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55159\source\repos\APSSystem_NOVO\src\APSSystem.Presentation.WPF\Data\Antecipacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D75A986-62DA-4878-8F98-8B1395E07609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C3F06A-5B17-43EE-8149-AD8549AFFA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34905" yWindow="5490" windowWidth="22320" windowHeight="15300" xr2:uid="{BE9E9A5A-8528-4279-9018-52A1C569EF13}"/>
+    <workbookView xWindow="26250" yWindow="15450" windowWidth="27855" windowHeight="16095" xr2:uid="{BE9E9A5A-8528-4279-9018-52A1C569EF13}"/>
   </bookViews>
   <sheets>
     <sheet name="machine" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>ASHE1</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>CAL-24x5</t>
-  </si>
-  <si>
-    <t>CAL-PADRAO-5x8</t>
   </si>
   <si>
     <t>Sliter 1</t>
@@ -81,7 +78,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -128,7 +125,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +445,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,13 +462,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -486,7 +483,7 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -494,7 +491,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>1000</v>
@@ -512,7 +509,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -520,7 +517,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>1000</v>
@@ -546,7 +543,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>1000</v>

</xml_diff>